<commit_message>
Changes of 14th June 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/src/TestFiles/CheetahProcessing_DEV.xlsx
+++ b/FedExApplication/src/TestFiles/CheetahProcessing_DEV.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="9660" tabRatio="614"/>
+    <workbookView tabRatio="614" windowHeight="9660" windowWidth="19815" xWindow="390" yWindow="510"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="140">
   <si>
     <t>Sno</t>
   </si>
@@ -248,6 +248,192 @@
   </si>
   <si>
     <t>320018799875</t>
+  </si>
+  <si>
+    <t>310109785247</t>
+  </si>
+  <si>
+    <t>310109785258</t>
+  </si>
+  <si>
+    <t>310109785280</t>
+  </si>
+  <si>
+    <t>310109785306</t>
+  </si>
+  <si>
+    <t>310109785340</t>
+  </si>
+  <si>
+    <t>310109785361</t>
+  </si>
+  <si>
+    <t>310109785394</t>
+  </si>
+  <si>
+    <t>310109785410</t>
+  </si>
+  <si>
+    <t>310109785442</t>
+  </si>
+  <si>
+    <t>310109785464</t>
+  </si>
+  <si>
+    <t>310109785501</t>
+  </si>
+  <si>
+    <t>310109785523</t>
+  </si>
+  <si>
+    <t>310109785556</t>
+  </si>
+  <si>
+    <t>310109785578</t>
+  </si>
+  <si>
+    <t>310109785659</t>
+  </si>
+  <si>
+    <t>310109785660</t>
+  </si>
+  <si>
+    <t>310109785692</t>
+  </si>
+  <si>
+    <t>310109785718</t>
+  </si>
+  <si>
+    <t>310109785751</t>
+  </si>
+  <si>
+    <t>310109785773</t>
+  </si>
+  <si>
+    <t>310109785800</t>
+  </si>
+  <si>
+    <t>310109785957</t>
+  </si>
+  <si>
+    <t>310109785968</t>
+  </si>
+  <si>
+    <t>310109785990</t>
+  </si>
+  <si>
+    <t>310109786026</t>
+  </si>
+  <si>
+    <t>310109786060</t>
+  </si>
+  <si>
+    <t>310109786081</t>
+  </si>
+  <si>
+    <t>310109786118</t>
+  </si>
+  <si>
+    <t>310109786130</t>
+  </si>
+  <si>
+    <t>310109786162</t>
+  </si>
+  <si>
+    <t>310109786184</t>
+  </si>
+  <si>
+    <t>310109786221</t>
+  </si>
+  <si>
+    <t>310109786243</t>
+  </si>
+  <si>
+    <t>310109786276</t>
+  </si>
+  <si>
+    <t>310109786298</t>
+  </si>
+  <si>
+    <t>310109786324</t>
+  </si>
+  <si>
+    <t>310109786346</t>
+  </si>
+  <si>
+    <t>310109786380</t>
+  </si>
+  <si>
+    <t>310109786405</t>
+  </si>
+  <si>
+    <t>310109786438</t>
+  </si>
+  <si>
+    <t>310109786450</t>
+  </si>
+  <si>
+    <t>310109786482</t>
+  </si>
+  <si>
+    <t>310109786493</t>
+  </si>
+  <si>
+    <t>310109786520</t>
+  </si>
+  <si>
+    <t>310109786541</t>
+  </si>
+  <si>
+    <t>310109786585</t>
+  </si>
+  <si>
+    <t>310109786600</t>
+  </si>
+  <si>
+    <t>310109786633</t>
+  </si>
+  <si>
+    <t>310109786655</t>
+  </si>
+  <si>
+    <t>310109786688</t>
+  </si>
+  <si>
+    <t>310109786703</t>
+  </si>
+  <si>
+    <t>310109786747</t>
+  </si>
+  <si>
+    <t>310109786769</t>
+  </si>
+  <si>
+    <t>310109786791</t>
+  </si>
+  <si>
+    <t>310109786817</t>
+  </si>
+  <si>
+    <t>310109786840</t>
+  </si>
+  <si>
+    <t>310109786861</t>
+  </si>
+  <si>
+    <t>310109786909</t>
+  </si>
+  <si>
+    <t>310109786920</t>
+  </si>
+  <si>
+    <t>310109786953</t>
+  </si>
+  <si>
+    <t>310109786975</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -352,49 +538,49 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="2" numFmtId="164" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -408,10 +594,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -569,7 +755,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -578,13 +764,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -594,7 +780,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -603,7 +789,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -612,7 +798,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -622,12 +808,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -658,7 +844,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -677,7 +863,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -689,7 +875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -698,33 +884,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="104.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="104.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="39">
+    <row ht="39" r="1" spans="1:30">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -824,7 +1010,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -837,19 +1023,19 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M2" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O2" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P2" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
@@ -866,7 +1052,7 @@
       <c r="AC2" s="11"/>
       <c r="AD2" s="11"/>
     </row>
-    <row r="3" spans="1:30" ht="14.25" customHeight="1">
+    <row customHeight="1" ht="14.25" r="3" spans="1:30">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -874,7 +1060,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -892,7 +1078,7 @@
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -916,7 +1102,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -932,20 +1118,20 @@
       </c>
       <c r="L4" s="11"/>
       <c r="M4" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N4" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O4" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P4" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q4" s="11"/>
       <c r="R4" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
@@ -968,10 +1154,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -986,21 +1172,21 @@
       </c>
       <c r="L5" s="11"/>
       <c r="M5" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O5" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P5" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
       <c r="S5" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
@@ -1022,10 +1208,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1041,24 +1227,24 @@
         <v>45</v>
       </c>
       <c r="L6" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M6" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N6" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O6" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P6" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q6" s="11"/>
       <c r="R6" s="11"/>
       <c r="S6" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="T6" t="s">
         <v>55</v>
@@ -1080,10 +1266,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1097,25 +1283,25 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M7" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N7" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O7" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P7" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="U7" t="s">
         <v>55</v>
@@ -1144,7 +1330,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -1200,7 +1386,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -1240,7 +1426,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -1280,7 +1466,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -1320,7 +1506,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -1362,10 +1548,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1379,26 +1565,26 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M13" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N13" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O13" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P13" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
       <c r="T13" s="11"/>
       <c r="U13" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="V13" s="11"/>
       <c r="W13" s="11"/>
@@ -1416,10 +1602,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1433,19 +1619,19 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M14" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N14" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O14" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P14" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
@@ -1453,7 +1639,7 @@
       <c r="T14" s="11"/>
       <c r="U14" s="11"/>
       <c r="V14" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="W14" s="11"/>
       <c r="X14" s="11"/>
@@ -1470,10 +1656,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1487,19 +1673,19 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M15" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N15" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O15" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P15" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q15" s="11"/>
       <c r="R15" s="11"/>
@@ -1508,7 +1694,7 @@
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
       <c r="W15" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="X15" s="11"/>
       <c r="Y15" s="11"/>
@@ -1524,10 +1710,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1541,19 +1727,19 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M16" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N16" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O16" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P16" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
@@ -1563,7 +1749,7 @@
       <c r="V16" s="11"/>
       <c r="W16" s="11"/>
       <c r="X16" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Y16" s="11"/>
       <c r="Z16" s="11"/>
@@ -1578,10 +1764,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1595,19 +1781,19 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M17" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N17" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O17" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P17" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
@@ -1618,7 +1804,7 @@
       <c r="W17" s="11"/>
       <c r="X17" s="11"/>
       <c r="Y17" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Z17" s="11"/>
       <c r="AA17" s="11"/>
@@ -1632,7 +1818,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -1674,7 +1860,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -1689,19 +1875,19 @@
         <v>42</v>
       </c>
       <c r="L19" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M19" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N19" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O19" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P19" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
@@ -1715,7 +1901,7 @@
       <c r="Z19" s="11"/>
       <c r="AA19" s="11"/>
       <c r="AB19" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="AC19" s="11"/>
       <c r="AD19" s="11"/>
@@ -1726,7 +1912,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>137</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -1741,19 +1927,19 @@
         <v>43</v>
       </c>
       <c r="L20" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M20" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N20" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O20" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P20" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
@@ -1768,7 +1954,7 @@
       <c r="AA20" s="11"/>
       <c r="AB20" s="11"/>
       <c r="AC20" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="AD20" s="11"/>
     </row>
@@ -1778,7 +1964,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>138</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -1793,19 +1979,19 @@
         <v>44</v>
       </c>
       <c r="L21" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="M21" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="N21" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="O21" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="P21" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
@@ -1821,10 +2007,10 @@
       <c r="AB21" s="11"/>
       <c r="AC21" s="11"/>
       <c r="AD21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" ht="26.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row ht="26.25" r="22" spans="1:30">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1866,7 +2052,7 @@
       <c r="AC22" s="11"/>
       <c r="AD22" s="11"/>
     </row>
-    <row r="23" spans="1:30" ht="26.25">
+    <row ht="26.25" r="23" spans="1:30">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1937,7 +2123,7 @@
       <c r="AD24" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>